<commit_message>
- Updating spring version - Updating vaadin version - Improved redis example - Adding advise example - Minor refactor for filters - Updated Reports Methods to work with the Vaadin's downloadhandler - Updated spring security settings
</commit_message>
<xml_diff>
--- a/backend-java-frontend-vaadin/src/main/resources/templates/excel/reportTemplate.xlsx
+++ b/backend-java-frontend-vaadin/src/main/resources/templates/excel/reportTemplate.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Work\Projects\framework-showcase\src\main\resources\templates\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Work\Projects\framework-showcase\backend-java-frontend-vaadin\src\main\resources\templates\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A90C3AE5-4CB7-41A7-B40A-40BA185B864E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E987606-270E-4E55-A969-DA97E44EFC36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Datos" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -116,9 +116,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
-  </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -247,7 +244,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -255,26 +252,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="3" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="3" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
@@ -563,29 +561,29 @@
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="42.5703125" customWidth="1"/>
-    <col min="2" max="3" width="25.28515625" customWidth="1"/>
-    <col min="4" max="4" width="97.5703125" customWidth="1"/>
-    <col min="5" max="5" width="22.85546875" customWidth="1"/>
-    <col min="6" max="6" width="25.28515625" customWidth="1"/>
-    <col min="7" max="7" width="42.28515625" customWidth="1"/>
+    <col min="1" max="1" width="42.54296875" customWidth="1"/>
+    <col min="2" max="3" width="25.26953125" customWidth="1"/>
+    <col min="4" max="4" width="97.54296875" customWidth="1"/>
+    <col min="5" max="5" width="22.81640625" customWidth="1"/>
+    <col min="6" max="6" width="25.26953125" customWidth="1"/>
+    <col min="7" max="7" width="42.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="20" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="9" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2"/>
@@ -595,8 +593,8 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="2"/>
@@ -606,42 +604,42 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
     </row>
-    <row r="6" spans="1:7" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+    <row r="6" spans="1:7" s="1" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="4" t="s">
         <v>6</v>
       </c>
       <c r="E6"/>
       <c r="F6"/>
       <c r="G6"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="8" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>